<commit_message>
fixes in file headings
</commit_message>
<xml_diff>
--- a/Words.xlsx
+++ b/Words.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yasar\Downloads\Cambridge_1_to_12\IELTS Words\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C06C06F8-6EBC-4E8C-8FC3-B105A033A7AF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{552FC724-C60F-4DDB-A226-64D40418BD3D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{55E5C695-D557-40B8-98B4-02D364C176D3}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>assess</t>
   </si>
@@ -74,6 +73,15 @@
   </si>
   <si>
     <t>yazışma</t>
+  </si>
+  <si>
+    <t>WORDS</t>
+  </si>
+  <si>
+    <t>TYPE</t>
+  </si>
+  <si>
+    <t>TR</t>
   </si>
 </sst>
 </file>
@@ -425,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D046C81C-C5B5-432C-9584-EBF4638CDA29}">
-  <dimension ref="B2:E6"/>
+  <dimension ref="B1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -438,6 +446,17 @@
     <col min="5" max="5" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>

</xml_diff>